<commit_message>
:recycle: refactor: Refatoracao do exercicio de 17
</commit_message>
<xml_diff>
--- a/tarefa 1 java/out/production/tarefa 1 java/TesteDeMesa.xlsx
+++ b/tarefa 1 java/out/production/tarefa 1 java/TesteDeMesa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEV\fatec\linguagemprogramacao I\fatec-linguagem-programacaoI\tarefa 1 java\ExercicioJava\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E836A491-E808-40F2-B307-E9957F16F22A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E3DE63-0DB4-410C-8D8C-26F1C832B062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10296" xr2:uid="{560F5334-DC9D-4D50-B0F2-1BB9E85C1802}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="98">
   <si>
     <t>Teste de Mesa Exercicios Java - Linguagem Programação I</t>
   </si>
@@ -301,9 +301,6 @@
     <t>max</t>
   </si>
   <si>
-    <t>fator</t>
-  </si>
-  <si>
     <t>api</t>
   </si>
   <si>
@@ -329,9 +326,6 @@
   </si>
   <si>
     <t>3.7</t>
-  </si>
-  <si>
-    <t>1.5</t>
   </si>
   <si>
     <t>7.2</t>
@@ -428,11 +422,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -445,13 +445,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -767,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38B4C00A-5BE3-4BDE-A689-F877F31F2066}">
-  <dimension ref="A1:J82"/>
+  <dimension ref="A1:I82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="G75" sqref="G75"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="G84" sqref="G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -786,22 +779,22 @@
     <col min="9" max="9" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -815,7 +808,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -829,12 +822,12 @@
         <v>680</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -856,9 +849,8 @@
       <c r="G8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>20000</v>
       </c>
@@ -880,14 +872,13 @@
       <c r="G9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -898,7 +889,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>1000</v>
       </c>
@@ -909,12 +900,12 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -1002,10 +993,10 @@
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="5"/>
+      <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
@@ -1145,10 +1136,10 @@
       <c r="C48" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E48" s="5"/>
+      <c r="E48" s="7"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
@@ -1192,12 +1183,12 @@
       <c r="B53" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="5"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="7"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
@@ -1220,12 +1211,12 @@
       <c r="B55" s="1">
         <v>4</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="5"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="7"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
@@ -1234,12 +1225,12 @@
       <c r="B56" s="1">
         <v>6</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D56" s="4"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="5"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="7"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
@@ -1253,12 +1244,12 @@
       <c r="B59" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="5"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="7"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
@@ -1281,12 +1272,12 @@
       <c r="B61" s="1">
         <v>4</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="5"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="7"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
@@ -1295,32 +1286,32 @@
       <c r="B62" s="1">
         <v>6</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C62" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="5"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="7"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C65" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D65" s="4"/>
-      <c r="E65" s="5"/>
-    </row>
-    <row r="66" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="D65" s="6"/>
+      <c r="E65" s="7"/>
+    </row>
+    <row r="66" spans="1:9" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>11</v>
       </c>
@@ -1333,7 +1324,7 @@
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>13</v>
       </c>
@@ -1346,12 +1337,12 @@
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>74</v>
       </c>
@@ -1362,7 +1353,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>160</v>
       </c>
@@ -1373,7 +1364,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>170</v>
       </c>
@@ -1384,12 +1375,12 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>77</v>
       </c>
@@ -1406,7 +1397,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>15000</v>
       </c>
@@ -1423,137 +1414,125 @@
         <v>18333.330000000002</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A79" s="9" t="s">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A79" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B79" s="9" t="s">
+      <c r="B79" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C79" s="9" t="s">
+      <c r="C79" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D79" s="9" t="s">
+      <c r="D79" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E79" s="9" t="s">
+      <c r="E79" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="F79" s="9" t="s">
+      <c r="F79" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G79" s="9" t="s">
+      <c r="G79" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I79" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="H79" s="9" t="s">
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A80" s="4">
+        <v>8</v>
+      </c>
+      <c r="B80" s="4">
+        <v>6</v>
+      </c>
+      <c r="C80" s="4">
+        <v>8</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E80" s="4">
+        <v>1</v>
+      </c>
+      <c r="F80" s="4">
+        <v>8</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H80" s="4">
+        <v>0</v>
+      </c>
+      <c r="I80" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="I79" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="J79" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A80" s="9">
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81" s="4">
         <v>8</v>
       </c>
-      <c r="B80" s="9">
+      <c r="B81" s="4">
         <v>6</v>
       </c>
-      <c r="C80" s="9">
+      <c r="C81" s="4">
+        <v>7</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E81" s="4">
+        <v>1</v>
+      </c>
+      <c r="F81" s="4">
+        <v>3</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H81" s="4">
+        <v>5</v>
+      </c>
+      <c r="I81" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82" s="4">
+        <v>5</v>
+      </c>
+      <c r="B82" s="4">
+        <v>6</v>
+      </c>
+      <c r="C82" s="4">
+        <v>4</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E82" s="4">
+        <v>0</v>
+      </c>
+      <c r="F82" s="4">
+        <v>0</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H82" s="4">
         <v>8</v>
       </c>
-      <c r="D80" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="E80" s="9">
-        <v>1.69</v>
-      </c>
-      <c r="F80" s="9">
-        <v>1</v>
-      </c>
-      <c r="G80" s="9">
-        <v>8</v>
-      </c>
-      <c r="H80" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I80" s="9">
-        <v>0</v>
-      </c>
-      <c r="J80" s="9" t="s">
+      <c r="I82" s="4" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A81" s="9">
-        <v>8</v>
-      </c>
-      <c r="B81" s="9">
-        <v>6</v>
-      </c>
-      <c r="C81" s="9">
-        <v>7</v>
-      </c>
-      <c r="D81" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="E81" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="F81" s="9">
-        <v>1</v>
-      </c>
-      <c r="G81" s="9">
-        <v>3</v>
-      </c>
-      <c r="H81" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I81" s="9">
-        <v>5</v>
-      </c>
-      <c r="J81" s="9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A82" s="9">
-        <v>5</v>
-      </c>
-      <c r="B82" s="9">
-        <v>6</v>
-      </c>
-      <c r="C82" s="9">
-        <v>4</v>
-      </c>
-      <c r="D82" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="E82" s="9">
-        <v>0</v>
-      </c>
-      <c r="F82" s="9">
-        <v>0</v>
-      </c>
-      <c r="G82" s="9">
-        <v>0</v>
-      </c>
-      <c r="H82" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I82" s="9">
-        <v>8</v>
-      </c>
-      <c r="J82" s="9" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>